<commit_message>
product app created and updated
</commit_message>
<xml_diff>
--- a/documents/Webtech MERN - Apr 2021.xlsx
+++ b/documents/Webtech MERN - Apr 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\mindtree-april2021\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EBE391-4FD3-4BFB-9296-7A85D19DEA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7970C0EA-4F53-48A2-9CDF-5AD225A6E1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1846,8 +1846,8 @@
   <dimension ref="A1:BF31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD8"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
codes, assignments, links and notes updated
</commit_message>
<xml_diff>
--- a/documents/Webtech MERN - Apr 2021.xlsx
+++ b/documents/Webtech MERN - Apr 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\mindtree-april2021\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3DAF7A-F2EA-4E41-A271-E36A9B8D1359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB8AC48-14B6-4AC0-A082-8367A16F71C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2126,9 +2126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
assignment and assignment plan uploaded
</commit_message>
<xml_diff>
--- a/documents/Webtech MERN - Apr 2021.xlsx
+++ b/documents/Webtech MERN - Apr 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\mindtree-april2021\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCE40DA-24D2-4953-ABFD-A4667BD1C91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2D0FA7-4A10-4FC3-B10E-492BCB9B8B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,22 +38,7 @@
     <author>ghosh</author>
   </authors>
   <commentList>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{9BF4976F-C4B2-4827-844B-8F6A304311AD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>no code found in assignment-5 zip (es6/7)
-no code uploaded for es6/7 OOP concepts
-no code for webpack uploaded</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{3F02A748-1B67-4BB4-B8DD-B1743FE97FC1}">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{6CCB859B-CF16-44F7-A3A5-6968E6521973}">
       <text>
         <r>
           <rPr>
@@ -61,9 +46,124 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>no code for webpack uploaded</t>
+          <t>code has been uploaded but is incomplete</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{ECDFB432-0397-4087-BED2-AD02DBAF0483}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>having compilation issues</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{76FF87A6-8363-4512-BEED-9C7B7F47454A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>having compilation issues</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{9E7C5583-CC70-4E75-8446-6ABDC90276F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>webpack assignment not uploaded</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{EE5FE9C7-920A-4D78-A3D3-015B5097B7A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SCSS assignment lacks lots of features like variable declaration, inheritance, include etc.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{7131CFC9-B531-4DF6-8CAC-2FD6A6B2FD31}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>SCSS assignment lacks lots of features like variable declaration, inheritance, include etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{3D88660D-7D06-4204-97AB-7D42E5E75FE2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">having compilation issues
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{2671BF53-A0E0-41D6-ABA6-0BB12ED81A69}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>not applying same style to alternate rows</t>
         </r>
       </text>
     </comment>
@@ -72,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="423">
   <si>
     <t>https://redux-saga.js.org/docs/introduction/BeginnerTutorial.html</t>
   </si>
@@ -1428,6 +1528,15 @@
   </si>
   <si>
     <t>M1067052</t>
+  </si>
+  <si>
+    <t>DOM-1</t>
+  </si>
+  <si>
+    <t>WebComponents</t>
+  </si>
+  <si>
+    <t>DOM-2</t>
   </si>
 </sst>
 </file>
@@ -1499,14 +1608,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -1600,7 +1709,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1642,37 +1751,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1681,7 +1773,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1832,13 +1924,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2196,9 +2290,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12:BG12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7058,10 +7152,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983E95EF-2C32-42F8-9CAB-F38FB8CA9197}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7071,9 +7165,14 @@
     <col min="3" max="3" width="44.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>393</v>
       </c>
@@ -7098,20 +7197,40 @@
       <c r="H1" s="41" t="s">
         <v>382</v>
       </c>
+      <c r="I1" s="59" t="s">
+        <v>420</v>
+      </c>
+      <c r="J1" s="59" t="s">
+        <v>421</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>422</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="59" t="s">
+        <v>201</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
         <v>397</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="38">
         <v>1</v>
       </c>
@@ -7136,8 +7255,13 @@
       <c r="H3" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>2</v>
       </c>
@@ -7156,14 +7280,19 @@
       <c r="F4" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="G4" s="57" t="s">
-        <v>392</v>
-      </c>
-      <c r="H4" s="57" t="s">
-        <v>392</v>
-      </c>
+      <c r="G4" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="38">
         <v>3</v>
       </c>
@@ -7188,8 +7317,13 @@
       <c r="H5" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="38">
         <v>4</v>
       </c>
@@ -7214,8 +7348,13 @@
       <c r="H6" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="38">
         <v>5</v>
       </c>
@@ -7234,26 +7373,36 @@
       <c r="F7" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="G7" s="57" t="s">
-        <v>392</v>
-      </c>
-      <c r="H7" s="57" t="s">
-        <v>392</v>
-      </c>
+      <c r="G7" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="58" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="62" t="s">
         <v>398</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="38">
         <v>6</v>
       </c>
@@ -7278,8 +7427,13 @@
       <c r="H9" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="38">
         <v>7</v>
       </c>
@@ -7304,8 +7458,13 @@
       <c r="H10" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="38">
         <v>8</v>
       </c>
@@ -7330,8 +7489,13 @@
       <c r="H11" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="38">
         <v>9</v>
       </c>
@@ -7356,8 +7520,13 @@
       <c r="H12" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="38">
         <v>10</v>
       </c>
@@ -7367,35 +7536,45 @@
       <c r="C13" s="47" t="s">
         <v>407</v>
       </c>
-      <c r="D13" s="39" t="s">
-        <v>392</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>392</v>
+      <c r="D13" s="42" t="s">
+        <v>394</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>394</v>
       </c>
       <c r="F13" s="39" t="s">
         <v>392</v>
       </c>
-      <c r="G13" s="57" t="s">
-        <v>392</v>
-      </c>
-      <c r="H13" s="57" t="s">
-        <v>392</v>
-      </c>
+      <c r="G13" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="H13" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="58" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="62" t="s">
         <v>399</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="60"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="38">
         <v>11</v>
       </c>
@@ -7420,8 +7599,13 @@
       <c r="H15" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="38">
         <v>12</v>
       </c>
@@ -7437,7 +7621,7 @@
       <c r="E16" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="57" t="s">
         <v>392</v>
       </c>
       <c r="G16" s="57" t="s">
@@ -7446,8 +7630,13 @@
       <c r="H16" s="57" t="s">
         <v>392</v>
       </c>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="38">
         <v>13</v>
       </c>
@@ -7472,8 +7661,13 @@
       <c r="H17" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="38">
         <v>14</v>
       </c>
@@ -7492,14 +7686,19 @@
       <c r="F18" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="G18" s="57" t="s">
-        <v>392</v>
-      </c>
-      <c r="H18" s="57" t="s">
-        <v>392</v>
-      </c>
+      <c r="G18" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="H18" s="58" t="s">
+        <v>394</v>
+      </c>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="38">
         <v>15</v>
       </c>
@@ -7524,12 +7723,17 @@
       <c r="H19" s="42" t="s">
         <v>394</v>
       </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A14:M14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:H7 D15:H19 D9:H13" xr:uid="{4CB5697C-CE9B-4D9C-AF2A-AE71901AAEC8}">

</xml_diff>